<commit_message>
AddressFormPage and MyAddressesPage created, testPlan updated
</commit_message>
<xml_diff>
--- a/data/testPlan.xlsx
+++ b/data/testPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Valid credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="49">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -64,94 +64,100 @@
     <t>Login with valid credentials</t>
   </si>
   <si>
+    <t>An already registered account</t>
+  </si>
+  <si>
+    <t>Navigate to webpage</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php</t>
+  </si>
+  <si>
+    <t>Webpage is open, sign in button is visible</t>
+  </si>
+  <si>
+    <t>As expected</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Click "Sign in" button</t>
+  </si>
+  <si>
+    <t>The button is clicked, the user is redirected to the login page</t>
+  </si>
+  <si>
+    <t>Enter valid email address</t>
+  </si>
+  <si>
+    <t>fakemail777@mailinator.com</t>
+  </si>
+  <si>
+    <t>Email is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter valid password</t>
+  </si>
+  <si>
+    <t>pass777</t>
+  </si>
+  <si>
+    <t>Password is entered and covered with asterisks</t>
+  </si>
+  <si>
+    <t>Sign out</t>
+  </si>
+  <si>
+    <t>User is logged in, my account page is visible, "Sign out" button is visible</t>
+  </si>
+  <si>
+    <t>LOG002</t>
+  </si>
+  <si>
+    <t>Login with invalid credentials</t>
+  </si>
+  <si>
+    <t>Enter invalid email address</t>
+  </si>
+  <si>
+    <t>fakemail888@mailinator.com</t>
+  </si>
+  <si>
+    <t>Enter invalid password</t>
+  </si>
+  <si>
+    <t>pass888</t>
+  </si>
+  <si>
+    <t>The user is not logged in, "Authentication failed" message is shown, the user is still on the login page</t>
+  </si>
+  <si>
+    <t>LOG003</t>
+  </si>
+  <si>
+    <t>Login with empty credentials</t>
+  </si>
+  <si>
+    <t>Leave email field empty</t>
+  </si>
+  <si>
+    <t>Email field is empty</t>
+  </si>
+  <si>
+    <t>Leave password field empty</t>
+  </si>
+  <si>
+    <t>Password field is empty</t>
+  </si>
+  <si>
+    <t>The user is not logged in, "An email address required" message is shown, the user is still on the login page</t>
+  </si>
+  <si>
+    <t>LOG004</t>
+  </si>
+  <si>
     <t>A valid account</t>
-  </si>
-  <si>
-    <t>Navigate to webpage</t>
-  </si>
-  <si>
-    <t>http://automationpractice.com/index.php</t>
-  </si>
-  <si>
-    <t>Webpage is open, sign in button is visible</t>
-  </si>
-  <si>
-    <t>As expected</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Click Sign in button</t>
-  </si>
-  <si>
-    <t>The button is clicked, the user is redirected to the login page</t>
-  </si>
-  <si>
-    <t>Enter valid email address</t>
-  </si>
-  <si>
-    <t>fakemail777@mailinator.com</t>
-  </si>
-  <si>
-    <t>Email is entered and visible</t>
-  </si>
-  <si>
-    <t>Enter valid password</t>
-  </si>
-  <si>
-    <t>pass777</t>
-  </si>
-  <si>
-    <t>Password is entered and covered with asterisks</t>
-  </si>
-  <si>
-    <t>Click "Sign in" button</t>
-  </si>
-  <si>
-    <t>Sign out</t>
-  </si>
-  <si>
-    <t>User is logged in, my account page is visible, "Sign out" button is visible</t>
-  </si>
-  <si>
-    <t>LOG002</t>
-  </si>
-  <si>
-    <t>Login with invalid credentials</t>
-  </si>
-  <si>
-    <t>fakemail888@mailinator.com</t>
-  </si>
-  <si>
-    <t>pass888</t>
-  </si>
-  <si>
-    <t>The user is not logged in, "Authentication failed" message is shown, the user is still on the login page</t>
-  </si>
-  <si>
-    <t>LOG003</t>
-  </si>
-  <si>
-    <t>Login with empty credentials</t>
-  </si>
-  <si>
-    <t>Leave email field empty</t>
-  </si>
-  <si>
-    <t>Email field is empty</t>
-  </si>
-  <si>
-    <t>Leave password field empty</t>
-  </si>
-  <si>
-    <t>Password field is empty</t>
-  </si>
-  <si>
-    <t>The user is not logged in, "An email address required" message is shown, the user is still on the login page</t>
-  </si>
-  <si>
-    <t>LOG004</t>
   </si>
   <si>
     <t>Click "Sign out" button</t>
@@ -165,10 +171,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -193,18 +199,26 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -223,6 +237,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -232,7 +254,22 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -247,14 +284,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -262,54 +300,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,7 +316,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,6 +328,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -346,25 +352,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,37 +514,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,115 +526,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,21 +543,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -590,11 +581,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,6 +601,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,17 +635,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,7 +648,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -660,134 +666,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -795,22 +801,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1133,8 +1142,8 @@
   <sheetPr/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1144,9 +1153,9 @@
     <col min="3" max="3" width="18.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="16.7777777777778" customWidth="1"/>
     <col min="5" max="5" width="13.8888888888889" customWidth="1"/>
-    <col min="6" max="6" width="16.8888888888889" customWidth="1"/>
+    <col min="6" max="6" width="11.3333333333333" customWidth="1"/>
     <col min="7" max="7" width="23.5555555555556" customWidth="1"/>
-    <col min="8" max="8" width="21.7777777777778" customWidth="1"/>
+    <col min="8" max="8" width="23.2222222222222" customWidth="1"/>
     <col min="9" max="9" width="21.3333333333333" customWidth="1"/>
     <col min="10" max="10" width="21.1111111111111" customWidth="1"/>
     <col min="11" max="11" width="9.66666666666667" customWidth="1"/>
@@ -1191,7 +1200,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="28.8" spans="1:12">
+    <row r="2" ht="43.2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1261,7 +1270,7 @@
       <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="8" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1311,13 +1320,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>19</v>
@@ -1395,7 +1404,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2"/>
@@ -1409,91 +1418,91 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1504,14 +1513,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
+    <col min="1" max="1" width="10.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="20.5555555555556" customWidth="1"/>
     <col min="4" max="4" width="19.2222222222222" customWidth="1"/>
     <col min="5" max="5" width="13.6666666666667" customWidth="1"/>
@@ -1523,7 +1533,7 @@
     <col min="12" max="12" width="11.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="43.2" spans="1:12">
+    <row r="1" ht="30" customHeight="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1561,15 +1571,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="43" customHeight="1" spans="1:12">
+    <row r="2" ht="43" customHeight="1" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1592,8 +1602,9 @@
         <v>20</v>
       </c>
       <c r="L2" s="2"/>
-    </row>
-    <row r="3" ht="43.2" spans="1:12">
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" ht="43.2" spans="1:13">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1616,8 +1627,9 @@
         <v>20</v>
       </c>
       <c r="L3" s="2"/>
-    </row>
-    <row r="4" ht="30" customHeight="1" spans="1:12">
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:13">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1627,9 +1639,9 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1642,8 +1654,9 @@
         <v>20</v>
       </c>
       <c r="L4" s="2"/>
-    </row>
-    <row r="5" ht="28.8" spans="1:12">
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" ht="28.8" spans="1:13">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1653,10 +1666,10 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>28</v>
@@ -1668,8 +1681,9 @@
         <v>20</v>
       </c>
       <c r="L5" s="2"/>
-    </row>
-    <row r="6" ht="77" customHeight="1" spans="1:12">
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" ht="77" customHeight="1" spans="1:13">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1679,11 +1693,11 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>19</v>
@@ -1692,8 +1706,9 @@
         <v>20</v>
       </c>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1706,8 +1721,9 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1720,8 +1736,9 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1734,6 +1751,49 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1747,20 +1807,22 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="25.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="3" max="3" width="24.7777777777778" customWidth="1"/>
     <col min="4" max="4" width="20.4444444444444" customWidth="1"/>
     <col min="5" max="5" width="12.8888888888889" customWidth="1"/>
-    <col min="6" max="6" width="8.33333333333333" customWidth="1"/>
+    <col min="6" max="6" width="8.55555555555556" customWidth="1"/>
     <col min="7" max="7" width="20.4444444444444" customWidth="1"/>
-    <col min="8" max="8" width="19.7777777777778" customWidth="1"/>
-    <col min="9" max="9" width="20.4444444444444" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="15.5555555555556" customWidth="1"/>
+    <col min="8" max="8" width="26.2222222222222" customWidth="1"/>
+    <col min="9" max="9" width="35.2222222222222" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="9.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="43.2" spans="1:12">
@@ -1801,15 +1863,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="28.8" spans="1:13">
+    <row r="2" ht="26.4" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1869,11 +1931,11 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>19</v>
@@ -1894,11 +1956,11 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>19</v>
@@ -1909,7 +1971,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" ht="75" customHeight="1" spans="1:13">
+    <row r="6" ht="45" customHeight="1" spans="1:13">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1919,11 +1981,11 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>19</v>
@@ -1935,63 +1997,63 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13">
@@ -2123,19 +2185,19 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="20.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="23.7777777777778" customWidth="1"/>
     <col min="5" max="5" width="15.1111111111111" customWidth="1"/>
     <col min="7" max="7" width="20.1111111111111" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="8" max="8" width="26.6666666666667" customWidth="1"/>
     <col min="9" max="9" width="23.6666666666667" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
@@ -2183,14 +2245,14 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -2212,7 +2274,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" ht="61" customHeight="1" spans="1:12">
+    <row r="3" ht="45" customHeight="1" spans="1:12">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2248,7 +2310,7 @@
       <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -2298,13 +2360,11 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>19</v>
@@ -2314,22 +2374,141 @@
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="6:11">
+    <row r="7" spans="1:12">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="6">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="G7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
WishlistTests and PersonalInfoTests added
</commit_message>
<xml_diff>
--- a/data/testPlan.xlsx
+++ b/data/testPlan.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Valid credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Invalid credentials" sheetId="2" r:id="rId2"/>
     <sheet name="Empty credentials" sheetId="3" r:id="rId3"/>
     <sheet name="Logout" sheetId="4" r:id="rId4"/>
+    <sheet name="Add address" sheetId="5" r:id="rId5"/>
+    <sheet name="Edit personal info" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="82">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -55,10 +57,10 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>TS001</t>
-  </si>
-  <si>
-    <t>LOG001</t>
+    <t>TS1</t>
+  </si>
+  <si>
+    <t>LOG1</t>
   </si>
   <si>
     <t>Login with valid credentials</t>
@@ -73,51 +75,54 @@
     <t>http://automationpractice.com/index.php</t>
   </si>
   <si>
+    <t>Webpage is open, the "Sign in" button is visible</t>
+  </si>
+  <si>
+    <t>As expected</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Click "Sign in" button</t>
+  </si>
+  <si>
+    <t>The button is clicked, the user is redirected to the login page</t>
+  </si>
+  <si>
+    <t>Enter valid email address</t>
+  </si>
+  <si>
+    <t>fakemail777@mailinator.com</t>
+  </si>
+  <si>
+    <t>Email is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter valid password</t>
+  </si>
+  <si>
+    <t>pass777</t>
+  </si>
+  <si>
+    <t>Password is entered and covered with asterisks</t>
+  </si>
+  <si>
+    <t>Sign out</t>
+  </si>
+  <si>
+    <t>User is logged in, my account page is visible, "Sign out" button is visible</t>
+  </si>
+  <si>
+    <t>LOG2</t>
+  </si>
+  <si>
+    <t>Login with invalid credentials</t>
+  </si>
+  <si>
     <t>Webpage is open, sign in button is visible</t>
   </si>
   <si>
-    <t>As expected</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Click "Sign in" button</t>
-  </si>
-  <si>
-    <t>The button is clicked, the user is redirected to the login page</t>
-  </si>
-  <si>
-    <t>Enter valid email address</t>
-  </si>
-  <si>
-    <t>fakemail777@mailinator.com</t>
-  </si>
-  <si>
-    <t>Email is entered and visible</t>
-  </si>
-  <si>
-    <t>Enter valid password</t>
-  </si>
-  <si>
-    <t>pass777</t>
-  </si>
-  <si>
-    <t>Password is entered and covered with asterisks</t>
-  </si>
-  <si>
-    <t>Sign out</t>
-  </si>
-  <si>
-    <t>User is logged in, my account page is visible, "Sign out" button is visible</t>
-  </si>
-  <si>
-    <t>LOG002</t>
-  </si>
-  <si>
-    <t>Login with invalid credentials</t>
-  </si>
-  <si>
     <t>Enter invalid email address</t>
   </si>
   <si>
@@ -133,7 +138,7 @@
     <t>The user is not logged in, "Authentication failed" message is shown, the user is still on the login page</t>
   </si>
   <si>
-    <t>LOG003</t>
+    <t>LOG3</t>
   </si>
   <si>
     <t>Login with empty credentials</t>
@@ -154,7 +159,10 @@
     <t>The user is not logged in, "An email address required" message is shown, the user is still on the login page</t>
   </si>
   <si>
-    <t>LOG004</t>
+    <t>LOG4</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
   <si>
     <t>A valid account</t>
@@ -164,6 +172,99 @@
   </si>
   <si>
     <t>User is logged out</t>
+  </si>
+  <si>
+    <t>TS2</t>
+  </si>
+  <si>
+    <t>ADD1</t>
+  </si>
+  <si>
+    <t>Add a new address</t>
+  </si>
+  <si>
+    <t>Click "Add a new address" button</t>
+  </si>
+  <si>
+    <t>User is redirected to the form page, a form is visible</t>
+  </si>
+  <si>
+    <t>Enter first name</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>First name is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter last name</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Last name is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter address</t>
+  </si>
+  <si>
+    <t>123 Bull Street</t>
+  </si>
+  <si>
+    <t>Address is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter city</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>City is entered and visible</t>
+  </si>
+  <si>
+    <t>Select state from a dropdown menu</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>The state is selected</t>
+  </si>
+  <si>
+    <t>Enter postal code</t>
+  </si>
+  <si>
+    <t>Postal code is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter mobile phone number</t>
+  </si>
+  <si>
+    <t>Mobile phone is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter address title</t>
+  </si>
+  <si>
+    <t>MyAddress2</t>
+  </si>
+  <si>
+    <t>Address title is entered and visible</t>
+  </si>
+  <si>
+    <t>Click "Save" button</t>
+  </si>
+  <si>
+    <t>The address is saved</t>
+  </si>
+  <si>
+    <t>Click "MY PERSONAL INFORMATION" button</t>
+  </si>
+  <si>
+    <t>Click "Mr" radio button</t>
   </si>
 </sst>
 </file>
@@ -171,10 +272,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -199,9 +300,30 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,38 +338,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,64 +352,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -336,8 +374,71 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,7 +453,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +477,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,7 +525,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,37 +537,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,37 +555,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,43 +585,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,13 +633,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,6 +644,54 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -557,26 +706,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -596,50 +730,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,7 +749,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -666,134 +767,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -810,15 +911,30 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1142,8 +1258,8 @@
   <sheetPr/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1153,11 +1269,11 @@
     <col min="3" max="3" width="18.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="16.7777777777778" customWidth="1"/>
     <col min="5" max="5" width="13.8888888888889" customWidth="1"/>
-    <col min="6" max="6" width="11.3333333333333" customWidth="1"/>
-    <col min="7" max="7" width="23.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="8.66666666666667" customWidth="1"/>
+    <col min="7" max="7" width="21.7777777777778" customWidth="1"/>
     <col min="8" max="8" width="23.2222222222222" customWidth="1"/>
     <col min="9" max="9" width="21.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="21.1111111111111" customWidth="1"/>
+    <col min="10" max="10" width="16.4444444444444" customWidth="1"/>
     <col min="11" max="11" width="9.66666666666667" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
   </cols>
@@ -1270,7 +1386,7 @@
       <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1404,7 +1520,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="7"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2"/>
@@ -1418,91 +1534,91 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="7"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1516,7 +1632,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1593,7 +1709,7 @@
         <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>19</v>
@@ -1602,7 +1718,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="5"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" ht="43.2" spans="1:13">
       <c r="A3" s="2"/>
@@ -1627,7 +1743,7 @@
         <v>20</v>
       </c>
       <c r="L3" s="2"/>
-      <c r="M3" s="5"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:13">
       <c r="A4" s="2"/>
@@ -1639,10 +1755,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>25</v>
@@ -1654,7 +1770,7 @@
         <v>20</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="M4" s="5"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" ht="28.8" spans="1:13">
       <c r="A5" s="2"/>
@@ -1666,10 +1782,10 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>28</v>
@@ -1681,7 +1797,7 @@
         <v>20</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="5"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" ht="77" customHeight="1" spans="1:13">
       <c r="A6" s="2"/>
@@ -1697,7 +1813,7 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>19</v>
@@ -1706,7 +1822,7 @@
         <v>20</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="5"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="2"/>
@@ -1721,7 +1837,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="2"/>
@@ -1736,7 +1852,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="5"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2"/>
@@ -1751,49 +1867,49 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="5"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1807,7 +1923,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1826,175 +1942,175 @@
   </cols>
   <sheetData>
     <row r="1" ht="43.2" spans="1:12">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" ht="26.4" spans="1:13">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3">
+      <c r="C2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" ht="51" customHeight="1" spans="1:13">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3">
+      <c r="I2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="11"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:13">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="7"/>
+      <c r="J3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="11"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="G4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="7"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" ht="28.8" spans="1:13">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12">
         <v>4</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
+      <c r="G5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="7"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="11"/>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" ht="45" customHeight="1" spans="1:13">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12">
         <v>5</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="7"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="2"/>
@@ -2009,7 +2125,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="7"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="2"/>
@@ -2024,7 +2140,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="7"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2"/>
@@ -2039,7 +2155,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="7"/>
+      <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2"/>
@@ -2054,127 +2170,127 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="7"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2188,7 +2304,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2200,6 +2316,7 @@
     <col min="8" max="8" width="26.6666666666667" customWidth="1"/>
     <col min="9" max="9" width="23.6666666666667" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="12" max="12" width="10.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="43.2" spans="1:12">
@@ -2245,14 +2362,14 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -2264,7 +2381,7 @@
         <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>19</v>
@@ -2375,140 +2492,836 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9">
         <v>6</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
+      <c r="G7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="A1:L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="18.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="19.1111111111111" customWidth="1"/>
+    <col min="7" max="7" width="25.4444444444444" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="28.3333333333333" customWidth="1"/>
+    <col min="10" max="10" width="13.7777777777778" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="31" customHeight="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="28.8" spans="1:12">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="5"/>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" ht="43" customHeight="1" spans="1:12">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:12">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" ht="28" customHeight="1" spans="1:12">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" ht="31" customHeight="1" spans="1:12">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" ht="34" customHeight="1" spans="6:11">
+      <c r="F9" s="5">
+        <v>8</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="6:11">
+      <c r="F10" s="7">
+        <v>9</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="6">
+        <v>60007</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" ht="28.8" spans="6:11">
+      <c r="F11" s="7">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1680000000</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="6:11">
+      <c r="F12" s="7">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="6:11">
+      <c r="F13" s="7">
+        <v>12</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="6:11">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="6:11">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="21.1111111111111" customWidth="1"/>
+    <col min="4" max="4" width="21.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="16.2222222222222" customWidth="1"/>
+    <col min="6" max="6" width="9.44444444444444" customWidth="1"/>
+    <col min="7" max="7" width="28.8888888888889" customWidth="1"/>
+    <col min="8" max="8" width="26.1111111111111" customWidth="1"/>
+    <col min="9" max="9" width="21.3333333333333" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="43.2" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="28.8" spans="1:12">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" ht="43.2" spans="1:12">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" ht="28.8" spans="1:12">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" ht="28.8" spans="1:12">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" ht="57.6" spans="1:12">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" ht="28.8" spans="1:12">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="6:11">
+      <c r="F9" s="5">
+        <v>8</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="6:11">
+      <c r="F10" s="7">
+        <v>9</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="6:11">
+      <c r="F11" s="7">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="6:11">
+      <c r="F12" s="7">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="6:11">
+      <c r="F13" s="7">
+        <v>12</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="6:11">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="6:11">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
CartPage and CartTests added, testPlan updated
</commit_message>
<xml_diff>
--- a/data/testPlan.xlsx
+++ b/data/testPlan.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Address tests" sheetId="11" r:id="rId2"/>
     <sheet name="Wishlist tests" sheetId="9" r:id="rId3"/>
     <sheet name="Personal info tests" sheetId="10" r:id="rId4"/>
-    <sheet name="Scenarios" sheetId="12" r:id="rId5"/>
+    <sheet name="Cart tests" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="156">
   <si>
     <t>TEST SCENARIO ID</t>
   </si>
@@ -278,7 +278,7 @@
     <t>Delete address</t>
   </si>
   <si>
-    <t>Click "Delete" button</t>
+    <t>Click "Delete" button under the second address</t>
   </si>
   <si>
     <t>Alert message "Are you sure" shows up</t>
@@ -323,6 +323,9 @@
     <t>Add multiple wishlists</t>
   </si>
   <si>
+    <t>Enter another wishlist name</t>
+  </si>
+  <si>
     <t>WSH-3</t>
   </si>
   <si>
@@ -341,6 +344,12 @@
     <t>Wishlist is deleted</t>
   </si>
   <si>
+    <t>Repeat last two steps until all wishlists are deleted</t>
+  </si>
+  <si>
+    <t>No more wishlists</t>
+  </si>
+  <si>
     <t>TS-4</t>
   </si>
   <si>
@@ -404,22 +413,79 @@
     <t>Personal info update saved</t>
   </si>
   <si>
-    <t>TEST SCENARIO NAME</t>
-  </si>
-  <si>
-    <t>Verify login functionality</t>
-  </si>
-  <si>
-    <t>Verify address funcionality</t>
-  </si>
-  <si>
-    <t>TS-3</t>
-  </si>
-  <si>
-    <t>Verify wishlist funcionality</t>
-  </si>
-  <si>
-    <t>Verify editing personal information</t>
+    <t>TS-5</t>
+  </si>
+  <si>
+    <t>CRT-1</t>
+  </si>
+  <si>
+    <t>Add one product to cart</t>
+  </si>
+  <si>
+    <t>Scroll down until you see product 1</t>
+  </si>
+  <si>
+    <t>Product 1 button is visible</t>
+  </si>
+  <si>
+    <t>Hover over product 1</t>
+  </si>
+  <si>
+    <t>"Add to cart" button is visible</t>
+  </si>
+  <si>
+    <t>Click "Add to cart" button</t>
+  </si>
+  <si>
+    <t>Product added to cart</t>
+  </si>
+  <si>
+    <t>Click "X" to close popup</t>
+  </si>
+  <si>
+    <t>Popup is closed</t>
+  </si>
+  <si>
+    <t>CRT-2</t>
+  </si>
+  <si>
+    <t>Add one product to cart and increase quantity to three</t>
+  </si>
+  <si>
+    <t>Scroll down until you see product 2</t>
+  </si>
+  <si>
+    <t>Hover over product 2</t>
+  </si>
+  <si>
+    <t>Click "Proceed to checkout" button</t>
+  </si>
+  <si>
+    <t>User is redirected to shopping cart</t>
+  </si>
+  <si>
+    <t>Click plus button</t>
+  </si>
+  <si>
+    <t>Quantity changed to two</t>
+  </si>
+  <si>
+    <t>Quantity changed to three</t>
+  </si>
+  <si>
+    <t>CRT-3</t>
+  </si>
+  <si>
+    <t>Remove product from cart</t>
+  </si>
+  <si>
+    <t>Click cart icon</t>
+  </si>
+  <si>
+    <t>Click garbage can icon</t>
+  </si>
+  <si>
+    <t>Product is deleted, cart is empty</t>
   </si>
 </sst>
 </file>
@@ -427,10 +493,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -457,14 +523,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -477,9 +543,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -493,8 +558,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -503,21 +569,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -563,17 +614,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -585,8 +642,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,7 +680,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,109 +782,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,7 +812,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,43 +854,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,35 +876,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -882,11 +922,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -905,12 +960,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -931,127 +997,127 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1059,10 +1125,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1404,7 +1470,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1419,55 +1485,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" ht="16" customHeight="1" spans="1:7">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1478,23 +1544,23 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1506,10 +1572,10 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1521,77 +1587,77 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -1602,23 +1668,23 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1630,10 +1696,10 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
         <v>27</v>
       </c>
@@ -1645,77 +1711,77 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -1726,27 +1792,27 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
       <c r="E20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -1754,10 +1820,10 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
       <c r="E22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1769,77 +1835,77 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
       <c r="E23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1" t="s">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -1850,27 +1916,27 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="s">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -1878,10 +1944,10 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
       <c r="E30" s="4" t="s">
         <v>27</v>
       </c>
@@ -1893,77 +1959,77 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1" t="s">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -1974,36 +2040,36 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
       <c r="E36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1" t="s">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="2"/>
       <c r="G37" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
       <c r="E38" s="4" t="s">
         <v>39</v>
       </c>
@@ -2013,77 +2079,77 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
       <c r="E39" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1" t="s">
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1" t="s">
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1" t="s">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -2094,23 +2160,23 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
       <c r="E44" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1" t="s">
+      <c r="F44" s="2"/>
+      <c r="G44" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
       <c r="E45" s="4" t="s">
         <v>18</v>
       </c>
@@ -2122,10 +2188,10 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
       <c r="E46" s="4" t="s">
         <v>21</v>
       </c>
@@ -2137,28 +2203,28 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
       <c r="E47" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1" t="s">
+      <c r="F47" s="2"/>
+      <c r="G47" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1" t="s">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1" t="s">
+      <c r="F48" s="2"/>
+      <c r="G48" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2174,7 +2240,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2190,58 +2256,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="33" customHeight="1" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="4" t="s">
         <v>52</v>
       </c>
@@ -2252,10 +2318,10 @@
       </c>
     </row>
     <row r="4" ht="19" customHeight="1" spans="1:8">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
         <v>54</v>
       </c>
@@ -2265,15 +2331,15 @@
       <c r="G4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
         <v>58</v>
       </c>
@@ -2283,16 +2349,16 @@
       <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -2301,16 +2367,16 @@
       <c r="G6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="4">
@@ -2319,12 +2385,12 @@
       <c r="G7" s="4">
         <v>11000</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="5:8">
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F8" s="4">
@@ -2338,7 +2404,7 @@
       </c>
     </row>
     <row r="9" spans="5:8">
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -2352,7 +2418,7 @@
       </c>
     </row>
     <row r="10" spans="5:8">
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H10" t="s">
@@ -2360,58 +2426,58 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" ht="28.8" spans="1:8">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
         <v>78</v>
       </c>
@@ -2422,10 +2488,10 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
         <v>54</v>
       </c>
@@ -2435,15 +2501,15 @@
       <c r="G15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="4" t="s">
         <v>58</v>
       </c>
@@ -2453,16 +2519,16 @@
       <c r="G16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -2471,16 +2537,16 @@
       <c r="G17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F18" s="4">
@@ -2489,12 +2555,12 @@
       <c r="G18" s="4">
         <v>11000</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="19" spans="5:8">
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F19" s="4">
@@ -2508,7 +2574,7 @@
       </c>
     </row>
     <row r="20" spans="5:8">
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -2522,7 +2588,7 @@
       </c>
     </row>
     <row r="21" spans="5:8">
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H21" t="s">
@@ -2530,58 +2596,58 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" ht="28.8" spans="1:8">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+    <row r="25" ht="28.8" spans="1:8">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="4" t="s">
         <v>86</v>
       </c>
@@ -2592,61 +2658,61 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="4" t="s">
         <v>88</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="1"/>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="1"/>
+      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="5:7">
-      <c r="E30" s="1"/>
+      <c r="E30" s="2"/>
       <c r="F30" s="4"/>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="5:7">
-      <c r="E31" s="1"/>
+      <c r="E31" s="2"/>
       <c r="F31" s="4"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="5:5">
-      <c r="E32" s="1"/>
+      <c r="E32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2657,10 +2723,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2669,68 +2735,68 @@
     <col min="2" max="2" width="12.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="25.8888888888889" customWidth="1"/>
-    <col min="5" max="5" width="31.5555555555556" customWidth="1"/>
-    <col min="6" max="6" width="26.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="34.7777777777778" customWidth="1"/>
+    <col min="6" max="6" width="23.4444444444444" customWidth="1"/>
     <col min="7" max="7" width="30.4444444444444" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:10">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:10">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -2739,244 +2805,280 @@
       <c r="G3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:10">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:10">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" ht="31" customHeight="1" spans="1:10">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" ht="27" customHeight="1" spans="1:7">
-      <c r="A14" s="1" t="s">
+    <row r="18" ht="27" customHeight="1" spans="1:7">
+      <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="C18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" ht="28.8" spans="1:7">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
+    <row r="19" ht="28.8" spans="1:7">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
         <v>106</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" ht="28.8" spans="5:7">
+      <c r="E21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3007,165 +3109,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="33" customHeight="1" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>111</v>
+      <c r="E2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:8">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>112</v>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H4" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="5" ht="17" customHeight="1" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H5" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>122</v>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>126</v>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>127</v>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3177,56 +3279,368 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="41.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="17.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="11.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="37.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="23.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="42.8888888888889" customWidth="1"/>
+    <col min="6" max="6" width="24.7777777777778" customWidth="1"/>
+    <col min="7" max="7" width="29.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="32" customHeight="1" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B2" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C2" s="2" t="s">
         <v>133</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" ht="26.4" spans="1:7">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" ht="18" customHeight="1" spans="1:7">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7">
+      <c r="E7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" ht="28.8" spans="1:7">
+      <c r="A10" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" ht="26.4" spans="1:7">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="5:7">
+      <c r="E15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="5:7">
+      <c r="E16" t="s">
+        <v>148</v>
+      </c>
+      <c r="G16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7">
+      <c r="E17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" ht="26.4" spans="1:7">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7">
+      <c r="E25" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7">
+      <c r="E26" t="s">
+        <v>153</v>
+      </c>
+      <c r="G26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7">
+      <c r="E27" t="s">
+        <v>154</v>
+      </c>
+      <c r="G27" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Assertions and new WebElements, test cases updated
</commit_message>
<xml_diff>
--- a/data/testPlan.xlsx
+++ b/data/testPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="4"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login tests" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="167">
   <si>
     <t>TEST SCENARIO ID</t>
   </si>
@@ -41,6 +41,9 @@
     <t>EXPECTED RESULT</t>
   </si>
   <si>
+    <t>STATUS</t>
+  </si>
+  <si>
     <t>TS-1</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t>Chrome is open</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>Go to webpage</t>
   </si>
   <si>
@@ -290,6 +296,9 @@
     <t>Address is deleted</t>
   </si>
   <si>
+    <t>TS-3</t>
+  </si>
+  <si>
     <t>WSH-1</t>
   </si>
   <si>
@@ -320,7 +329,7 @@
     <t>WSH-2</t>
   </si>
   <si>
-    <t>Add multiple wishlists</t>
+    <t>Add 3 wishlists</t>
   </si>
   <si>
     <t>Enter another wishlist name</t>
@@ -425,6 +434,9 @@
     <t>Scroll down until you see product 1</t>
   </si>
   <si>
+    <t>Faded Short Sleeve T-shirts</t>
+  </si>
+  <si>
     <t>Product 1 button is visible</t>
   </si>
   <si>
@@ -440,40 +452,61 @@
     <t>Product added to cart</t>
   </si>
   <si>
+    <t>Click "Proceed to checkout" button</t>
+  </si>
+  <si>
+    <t>1 Product</t>
+  </si>
+  <si>
+    <t>User is redirected to shopping cart</t>
+  </si>
+  <si>
+    <t>CRT-2</t>
+  </si>
+  <si>
+    <t>Add one product to cart and increase quantity to three</t>
+  </si>
+  <si>
+    <t>Scroll down until you see product 2</t>
+  </si>
+  <si>
+    <t>Hover over product 2</t>
+  </si>
+  <si>
+    <t>Blouse</t>
+  </si>
+  <si>
+    <t>Click plus button</t>
+  </si>
+  <si>
+    <t>Quantity changed to two</t>
+  </si>
+  <si>
+    <t>Quantity changed to three</t>
+  </si>
+  <si>
+    <t>CRT-3</t>
+  </si>
+  <si>
+    <t>Add multiple products to cart</t>
+  </si>
+  <si>
     <t>Click "X" to close popup</t>
   </si>
   <si>
     <t>Popup is closed</t>
   </si>
   <si>
-    <t>CRT-2</t>
-  </si>
-  <si>
-    <t>Add one product to cart and increase quantity to three</t>
-  </si>
-  <si>
-    <t>Scroll down until you see product 2</t>
-  </si>
-  <si>
-    <t>Hover over product 2</t>
-  </si>
-  <si>
-    <t>Click "Proceed to checkout" button</t>
-  </si>
-  <si>
-    <t>User is redirected to shopping cart</t>
-  </si>
-  <si>
-    <t>Click plus button</t>
-  </si>
-  <si>
-    <t>Quantity changed to two</t>
-  </si>
-  <si>
-    <t>Quantity changed to three</t>
-  </si>
-  <si>
-    <t>CRT-3</t>
+    <t>Hover over product 3</t>
+  </si>
+  <si>
+    <t>Printed Dress</t>
+  </si>
+  <si>
+    <t>3 Products</t>
+  </si>
+  <si>
+    <t>CRT-4</t>
   </si>
   <si>
     <t>Remove product from cart</t>
@@ -493,10 +526,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -521,11 +554,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -536,15 +568,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -558,9 +584,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -574,11 +606,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -613,38 +667,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -659,7 +692,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -680,7 +713,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,31 +767,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,7 +791,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -740,25 +827,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,13 +845,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,37 +875,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -836,31 +887,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -874,11 +907,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -922,26 +970,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -976,7 +1009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -994,134 +1027,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1135,6 +1168,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1467,13 +1512,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="16.7777777777778" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -1484,7 +1529,7 @@
     <col min="7" max="7" width="26.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1506,97 +1551,118 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" ht="16" customHeight="1" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="16" customHeight="1" spans="1:8">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1608,7 +1674,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1630,97 +1696,118 @@
       <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1732,7 +1819,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1754,97 +1841,118 @@
       <c r="G17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1856,7 +1964,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1878,97 +1986,118 @@
       <c r="G25" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>19</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1980,7 +2109,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2002,93 +2131,114 @@
       <c r="G33" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2100,7 +2250,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -2122,110 +2272,134 @@
       <c r="G41" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>19</v>
+      </c>
+      <c r="H44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="H45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="H46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>26</v>
+      </c>
+      <c r="H47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="H48" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2237,13 +2411,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="13.1111111111111" customWidth="1"/>
@@ -2253,9 +2427,10 @@
     <col min="6" max="6" width="21.8888888888889" customWidth="1"/>
     <col min="7" max="7" width="22.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
+    <col min="9" max="9" width="8.55555555555556" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2272,112 +2447,130 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="33" customHeight="1" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="33" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" ht="19" customHeight="1" spans="1:8">
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="19" customHeight="1" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>63</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>67</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F7" s="4">
         <v>60007</v>
@@ -2386,46 +2579,58 @@
         <v>11000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="5:8">
+        <v>69</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9">
       <c r="E8" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F8" s="4">
         <v>1680000000</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="10">
         <v>680000000</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="5:8">
+        <v>71</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9">
       <c r="E9" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="5:8">
+        <v>75</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9">
       <c r="E10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>77</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -2442,112 +2647,130 @@
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" ht="28.8" spans="1:8">
+      <c r="I12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" ht="28.8" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>53</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>56</v>
+        <v>81</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>59</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>67</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F18" s="4">
         <v>12345</v>
@@ -2556,46 +2779,58 @@
         <v>11000</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8">
+        <v>69</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9">
       <c r="E19" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F19" s="4">
         <v>2680030050</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="10">
         <v>680000000</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="5:8">
+        <v>71</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9">
       <c r="E20" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>72</v>
+        <v>84</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="5:8">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9">
       <c r="E21" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>85</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2612,63 +2847,75 @@
         <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" ht="28.8" spans="1:8">
+      <c r="I23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" ht="28.8" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" ht="28.8" spans="1:8">
+        <v>53</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" ht="28.8" spans="1:9">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>89</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="I26" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2704,12 +2951,12 @@
     <row r="30" spans="5:7">
       <c r="E30" s="2"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="6"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="5:7">
       <c r="E31" s="2"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="5"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" s="2"/>
@@ -2723,10 +2970,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2738,7 +2985,7 @@
     <col min="5" max="5" width="34.7777777777778" customWidth="1"/>
     <col min="6" max="6" width="23.4444444444444" customWidth="1"/>
     <col min="7" max="7" width="30.4444444444444" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="8" max="8" width="7.77777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2763,31 +3010,35 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
@@ -2797,15 +3048,17 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
@@ -2815,13 +3068,15 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
@@ -2838,66 +3093,76 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="7" ht="31" customHeight="1" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" ht="31" customHeight="1" spans="1:10">
-      <c r="A8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
@@ -2906,70 +3171,81 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>94</v>
+      <c r="E9" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:8">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="4" t="s">
-        <v>97</v>
+      <c r="E10" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="4" t="s">
-        <v>97</v>
+      <c r="E12" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="4" t="s">
-        <v>96</v>
+      <c r="H13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2977,108 +3253,101 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" ht="27" customHeight="1" spans="1:8">
+      <c r="A16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" ht="27" customHeight="1" spans="1:7">
-      <c r="A18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="G16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" ht="28.8" spans="1:8">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" ht="28.8" spans="1:7">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" ht="28.8" spans="5:8">
       <c r="E19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" ht="28.8" spans="5:7">
-      <c r="E21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="G19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3090,25 +3359,25 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="12.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="22.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="26.7777777777778" customWidth="1"/>
     <col min="5" max="5" width="36.8888888888889" customWidth="1"/>
-    <col min="6" max="6" width="26.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="22.3333333333333" customWidth="1"/>
     <col min="7" max="7" width="25.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="31.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3125,149 +3394,176 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="33" customHeight="1" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="33" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1" spans="1:8">
+        <v>117</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" spans="1:9">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>119</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" ht="17" customHeight="1" spans="1:8">
+        <v>123</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="17" customHeight="1" spans="1:9">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>127</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>132</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3279,13 +3575,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="17.4444444444444" customWidth="1"/>
     <col min="2" max="2" width="11.7777777777778" customWidth="1"/>
@@ -3294,9 +3590,10 @@
     <col min="5" max="5" width="42.8888888888889" customWidth="1"/>
     <col min="6" max="6" width="24.7777777777778" customWidth="1"/>
     <col min="7" max="7" width="29.1111111111111" customWidth="1"/>
+    <col min="8" max="8" width="9.55555555555556" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3318,89 +3615,116 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="32" customHeight="1" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" ht="26.4" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="26.4" spans="1:8">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>139</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>140</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
       <c r="G5" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" ht="18" customHeight="1" spans="1:7">
+        <v>141</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" ht="18" customHeight="1" spans="1:8">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>142</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="5:7">
+        <v>143</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8">
       <c r="E7" t="s">
-        <v>140</v>
+        <v>144</v>
+      </c>
+      <c r="F7" t="s">
+        <v>145</v>
       </c>
       <c r="G7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>146</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -3422,108 +3746,137 @@
       <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" ht="28.8" spans="1:7">
+      <c r="H9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" ht="28.8" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" ht="26.4" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" ht="26.4" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>139</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>141</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>142</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="G14" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="5:7">
+        <v>143</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8">
       <c r="E15" t="s">
+        <v>144</v>
+      </c>
+      <c r="G15" t="s">
         <v>146</v>
       </c>
-      <c r="G15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="5:7">
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8">
       <c r="E16" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G16" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7">
+        <v>153</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8">
       <c r="E17" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F17">
         <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>154</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -3545,102 +3898,350 @@
       <c r="G19" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" ht="26.4" spans="1:8">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
+      <c r="G27" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8">
+      <c r="E29" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="5:8">
+      <c r="E30" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8">
+      <c r="E31" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G31" t="s">
+        <v>146</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" ht="26.4" spans="1:7">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" ht="26.4" spans="1:8">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4" t="s">
+      <c r="F35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2" t="s">
+      <c r="F36" s="3"/>
+      <c r="G36" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="25" spans="5:7">
-      <c r="E25" t="s">
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G25" t="s">
+      <c r="F37" s="3"/>
+      <c r="G37" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="26" spans="5:7">
-      <c r="E26" t="s">
-        <v>153</v>
-      </c>
-      <c r="G26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="5:7">
-      <c r="E27" t="s">
-        <v>154</v>
-      </c>
-      <c r="G27" t="s">
-        <v>155</v>
+      <c r="H37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="5:8">
+      <c r="E39" t="s">
+        <v>157</v>
+      </c>
+      <c r="G39" t="s">
+        <v>158</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="5:8">
+      <c r="E40" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40" t="s">
+        <v>146</v>
+      </c>
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="5:8">
+      <c r="E41" t="s">
+        <v>165</v>
+      </c>
+      <c r="G41" t="s">
+        <v>166</v>
+      </c>
+      <c r="H41" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>